<commit_message>
Actualización de solicitudes guion 5
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion05/Solicitud_Grafica_LE_08_05_REC110.xlsx
+++ b/fuentes/contenidos/grado08/guion05/Solicitud_Grafica_LE_08_05_REC110.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="199">
   <si>
     <t>Fecha:</t>
   </si>
@@ -607,12 +607,6 @@
     <t>LE_08_05_REC110</t>
   </si>
   <si>
-    <t>http://www.banrepcultural.org/node/86383</t>
-  </si>
-  <si>
-    <t>Contertulios del Café El Automático: Juan Lozano y Lozano, León de Greiff, Ignacio Gómez Jaramillo, Jorge Zalamea. Detrás: Omar Rayo, Hernán Merino, Marco Ospina, Hernando Téllez, Arturo Camacho Ramírez. Caricatura de Mardoqueo Montaña, 1966.</t>
-  </si>
-  <si>
     <t>SHUTTER: 193423694</t>
   </si>
   <si>
@@ -620,6 +614,21 @@
   </si>
   <si>
     <t>SHUTTER: 204675202</t>
+  </si>
+  <si>
+    <t>SHUTTER: 224415874</t>
+  </si>
+  <si>
+    <t>Vintage books sketch seamless pattern with bird feather tea cup and glasses vector illustration</t>
+  </si>
+  <si>
+    <t>cartoon people talking happily</t>
+  </si>
+  <si>
+    <t>People on phone, chatting, taking pictures, texting, etc.</t>
+  </si>
+  <si>
+    <t>Vector concept of creative teamwork with light bulb puzzle and human hands</t>
   </si>
 </sst>
 </file>
@@ -1781,66 +1790,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>459133</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>15364</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1718495</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>1336573</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="16820625" y="2166170"/>
-          <a:ext cx="1259362" cy="1321209"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -2555,9 +2504,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3:G3"/>
+      <selection pane="bottomLeft" activeCell="J19" sqref="J17:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2845,13 +2794,13 @@
         <v>M10B</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="11" customFormat="1" ht="108" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="11" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
       </c>
       <c r="B10" s="62" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C10" s="20" t="str">
         <f t="shared" ref="C10:C41" si="0">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
@@ -2879,10 +2828,10 @@
         <f ca="1">IF(OR($B10&lt;&gt;"",$J10&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E10,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E10,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 460 px</v>
       </c>
-      <c r="J10" s="63" t="s">
-        <v>192</v>
-      </c>
-      <c r="K10" s="64"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="64" t="s">
+        <v>195</v>
+      </c>
       <c r="O10" s="2" t="str">
         <f>'Definición técnica de imagenes'!A12</f>
         <v>M12D</v>
@@ -2894,7 +2843,7 @@
         <v>IMG02</v>
       </c>
       <c r="B11" s="62" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C11" s="20" t="str">
         <f t="shared" si="0"/>
@@ -2923,19 +2872,21 @@
         <v>800 x 460 px</v>
       </c>
       <c r="J11" s="64"/>
-      <c r="K11" s="65"/>
+      <c r="K11" s="65" t="s">
+        <v>196</v>
+      </c>
       <c r="O11" s="2" t="str">
         <f>'Definición técnica de imagenes'!A13</f>
         <v>M101</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG03</v>
       </c>
       <c r="B12" s="62" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C12" s="20" t="str">
         <f t="shared" si="0"/>
@@ -2964,19 +2915,21 @@
         <v>800 x 460 px</v>
       </c>
       <c r="J12" s="64"/>
-      <c r="K12" s="64"/>
+      <c r="K12" s="64" t="s">
+        <v>197</v>
+      </c>
       <c r="O12" s="2" t="str">
         <f>'Definición técnica de imagenes'!A18</f>
         <v>Diaporama F1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG04</v>
       </c>
       <c r="B13" s="62" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C13" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3005,7 +2958,9 @@
         <v>800 x 460 px</v>
       </c>
       <c r="J13" s="64"/>
-      <c r="K13" s="64"/>
+      <c r="K13" s="64" t="s">
+        <v>198</v>
+      </c>
       <c r="O13" s="2" t="str">
         <f>'Definición técnica de imagenes'!A19</f>
         <v>F4</v>
@@ -6046,7 +6001,6 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>